<commit_message>
Test to serch after value in range
</commit_message>
<xml_diff>
--- a/ExcelInterop/Assembly_time_calculator.xlsx
+++ b/ExcelInterop/Assembly_time_calculator.xlsx
@@ -5990,8 +5990,8 @@
   </sheetPr>
   <dimension ref="A1:BB1519"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61:J61"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6208,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="132" t="s">
-        <v>188</v>
+        <v>73</v>
       </c>
       <c r="D5" s="133"/>
       <c r="E5" s="26"/>
@@ -6239,7 +6239,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="134">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D6" s="135"/>
       <c r="E6" s="28"/>
@@ -6270,7 +6270,7 @@
         <v>187</v>
       </c>
       <c r="C7" s="134">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D7" s="135"/>
       <c r="E7" s="26"/>
@@ -6332,7 +6332,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="139" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9" s="140"/>
       <c r="E9" s="26"/>
@@ -6363,7 +6363,7 @@
         <v>79</v>
       </c>
       <c r="C10" s="139" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="D10" s="140"/>
       <c r="E10" s="26"/>
@@ -6394,7 +6394,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="139" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="D11" s="141"/>
       <c r="E11" s="26"/>
@@ -6446,7 +6446,7 @@
         <v>93</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="D13" s="135"/>
       <c r="E13" s="50"/>
@@ -6473,7 +6473,7 @@
         <v>210</v>
       </c>
       <c r="C14" s="121">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D14" s="122"/>
       <c r="E14" s="26"/>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="G39" s="72">
         <f>($I$119+$I$130+$I$150+$I$163+$I$193+$I$204+$I$219)+IF($C$13=$B$248,C7*2)</f>
-        <v>0</v>
+        <v>57.901333333333334</v>
       </c>
       <c r="H39" s="145" t="s">
         <v>28</v>
@@ -6997,7 +6997,7 @@
       <c r="I39" s="146"/>
       <c r="J39" s="151">
         <f>SUM(G39:G42)</f>
-        <v>0</v>
+        <v>76.485262333333338</v>
       </c>
       <c r="K39" s="75"/>
       <c r="L39" s="26"/>
@@ -7014,7 +7014,7 @@
       </c>
       <c r="G40" s="73">
         <f>$I$182</f>
-        <v>0</v>
+        <v>6.9986166666666669</v>
       </c>
       <c r="H40" s="147"/>
       <c r="I40" s="148"/>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="G41" s="74">
         <f>$I$173</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="H41" s="147"/>
       <c r="I41" s="148"/>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="G42" s="74">
         <f>($G$39+$G$40+$G$41)*10%</f>
-        <v>0</v>
+        <v>6.9532056666666682</v>
       </c>
       <c r="H42" s="149"/>
       <c r="I42" s="150"/>
@@ -7420,21 +7420,21 @@
       </c>
       <c r="E65" s="16">
         <f>IF(C5=B227,C6,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F65" s="76" t="s">
         <v>0</v>
       </c>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>468</v>
       </c>
       <c r="H65" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I65" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.8</v>
       </c>
       <c r="J65" s="16" t="s">
         <v>16</v>
@@ -7548,21 +7548,21 @@
       </c>
       <c r="E69" s="16">
         <f>IF(OR(C5=B227,C5=B228,),C7,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F69" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G69" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="H69" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I69" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J69" s="16" t="s">
         <v>16</v>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="E71" s="98">
         <f>((C6/C52*1000)*2+2)</f>
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="F71" s="76" t="s">
         <v>2</v>
@@ -7623,15 +7623,15 @@
       </c>
       <c r="H71" s="98">
         <f>IF(D52&lt;=0,E71)</f>
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="I71" s="19" t="b">
         <f>IF($D$16=$B$248,(G71+H71)*C71)</f>
         <v>0</v>
       </c>
-      <c r="J71" s="157" t="b">
+      <c r="J71" s="157">
         <f>IF(C9=C247,SUM(I71:I73))</f>
-        <v>0</v>
+        <v>1.2266666666666668</v>
       </c>
     </row>
     <row r="72" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7644,7 +7644,7 @@
       </c>
       <c r="E72" s="98">
         <f>IF(C11=B234,0,(((C6/C12)*1000)*2+2))</f>
-        <v>0</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="F72" s="76" t="s">
         <v>2</v>
@@ -7655,11 +7655,11 @@
       </c>
       <c r="H72" s="98">
         <f>IF(D12&lt;=0,E72)</f>
-        <v>0</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="I72" s="19">
         <f>IF($C$11=$B$234,0,(G72+H72)*C72)</f>
-        <v>0</v>
+        <v>1.2266666666666668</v>
       </c>
       <c r="J72" s="158"/>
     </row>
@@ -7673,17 +7673,17 @@
       </c>
       <c r="E73" s="98">
         <f>C6*C73</f>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F73" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G73" s="19">
         <f>(E73-I71-I72)</f>
-        <v>0</v>
+        <v>-2.6666666666666838E-2</v>
       </c>
       <c r="H73" s="26"/>
-      <c r="I73" s="97" t="b">
+      <c r="I73" s="97">
         <f>IF(G73&gt;0,G73,IF(G73&lt;0,0))</f>
         <v>0</v>
       </c>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="E74" s="98">
         <f>((C6/C52*1000)*2+2)</f>
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="F74" s="76" t="s">
         <v>2</v>
@@ -7712,7 +7712,7 @@
       </c>
       <c r="H74" s="98">
         <f>IF(D52&lt;=0,E74)</f>
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="I74" s="19" t="b">
         <f>IF($D$16=$B$248,(G74+H74)*C74)</f>
@@ -7733,7 +7733,7 @@
       </c>
       <c r="E75" s="98">
         <f>IF(C11=B234,0,(((C6/C12)*1000)*2+2))</f>
-        <v>0</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="F75" s="76" t="s">
         <v>2</v>
@@ -7744,11 +7744,11 @@
       </c>
       <c r="H75" s="98">
         <f>IF(D12&lt;=0,E75)</f>
-        <v>0</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="I75" s="19">
         <f>IF($C$11=$B$234,0,(G75+H75)*C75)</f>
-        <v>0</v>
+        <v>0.92</v>
       </c>
       <c r="J75" s="158"/>
     </row>
@@ -7762,19 +7762,19 @@
       </c>
       <c r="E76" s="98">
         <f>C6*C76</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G76" s="19">
         <f>(E76-I74-I75)</f>
-        <v>0</v>
+        <v>7.999999999999996E-2</v>
       </c>
       <c r="H76" s="26"/>
-      <c r="I76" s="97" t="b">
+      <c r="I76" s="97">
         <f>IF(G76&gt;0,G76,IF(G76&lt;0,0))</f>
-        <v>0</v>
+        <v>7.999999999999996E-2</v>
       </c>
       <c r="J76" s="159"/>
     </row>
@@ -7790,7 +7790,7 @@
       </c>
       <c r="E77" s="98">
         <f>((C6/C52*1000)*2+2)</f>
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="F77" s="76" t="s">
         <v>2</v>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="H77" s="98">
         <f>IF(D52&lt;=0,E77)</f>
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="I77" s="19" t="b">
         <f>IF($D$16=$B$248,(G77+H77)*C77)</f>
@@ -7822,7 +7822,7 @@
       </c>
       <c r="E78" s="98">
         <f>IF(C11=B234,0,(((C6/C12)*1000)*2+2))</f>
-        <v>0</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="F78" s="76" t="s">
         <v>2</v>
@@ -7833,11 +7833,11 @@
       </c>
       <c r="H78" s="98">
         <f>IF(D12&lt;=0,E78)</f>
-        <v>0</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="I78" s="19">
         <f>IF($C$11=$B$234,0,(G78+H78)*C78)</f>
-        <v>0</v>
+        <v>0.9966666666666667</v>
       </c>
       <c r="J78" s="158"/>
     </row>
@@ -7851,19 +7851,19 @@
       </c>
       <c r="E79" s="98">
         <f>C6*C79</f>
-        <v>0</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="F79" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G79" s="19">
         <f>(E79-I77-I78)</f>
-        <v>0</v>
+        <v>0.15333333333333343</v>
       </c>
       <c r="H79" s="26"/>
-      <c r="I79" s="97" t="b">
+      <c r="I79" s="97">
         <f>IF(G79&gt;0,G79,IF(G79&lt;0,0))</f>
-        <v>0</v>
+        <v>0.15333333333333343</v>
       </c>
       <c r="J79" s="159"/>
     </row>
@@ -7879,21 +7879,21 @@
       </c>
       <c r="E80" s="80">
         <f>C14</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F80" s="76" t="s">
         <v>2</v>
       </c>
       <c r="G80" s="81">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="H80" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I80" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J80" s="76" t="s">
         <v>16</v>
@@ -7911,14 +7911,14 @@
       </c>
       <c r="E81" s="16">
         <f>IF(C10=B248,C6,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F81" s="76" t="s">
         <v>0</v>
       </c>
       <c r="G81" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="H81" s="16" t="b">
         <f>IF(C5=B226,G81)</f>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="I81" s="19">
         <f>(G81+H81)/60</f>
-        <v>0</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="J81" s="76" t="s">
         <v>16</v>
@@ -8668,7 +8668,7 @@
       </c>
       <c r="E103" s="98">
         <f>($C6/3)</f>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="F103" s="98" t="e">
         <f>AVERAGE(J82:J101)</f>
@@ -9068,23 +9068,23 @@
       </c>
       <c r="E116" s="16">
         <f>EVEN(IF(C11=B235,(C6/C12)*1000,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F116" s="16">
         <f>IF(D12&lt;1,E116)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G116" s="16">
         <f>F116*C116</f>
-        <v>0</v>
-      </c>
-      <c r="H116" s="16" t="b">
+        <v>2.2080000000000002</v>
+      </c>
+      <c r="H116" s="16">
         <f>IF(C11=B235,D12*C116)</f>
         <v>0</v>
       </c>
       <c r="I116" s="19">
         <f>G116+H116</f>
-        <v>0</v>
+        <v>2.2080000000000002</v>
       </c>
       <c r="J116" s="16" t="s">
         <v>16</v>
@@ -9170,7 +9170,7 @@
       <c r="H119" s="15"/>
       <c r="I119" s="15">
         <f>SUM(I63:I70,J71:J79,I80:I81,I102:I103,I114:I118)</f>
-        <v>0</v>
+        <v>37.901333333333334</v>
       </c>
       <c r="J119" s="15" t="s">
         <v>17</v>
@@ -10399,21 +10399,21 @@
       </c>
       <c r="E168" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="F168" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G168" s="19">
         <f>E168*60</f>
-        <v>0</v>
+        <v>277.9264</v>
       </c>
       <c r="H168" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I168" s="19">
         <f>E168</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="J168" s="16" t="s">
         <v>16</v>
@@ -10431,21 +10431,21 @@
       </c>
       <c r="E169" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="F169" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G169" s="19">
         <f>E169*60</f>
-        <v>0</v>
+        <v>277.9264</v>
       </c>
       <c r="H169" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I169" s="19">
         <f>E169</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="J169" s="16" t="s">
         <v>16</v>
@@ -10463,21 +10463,21 @@
       </c>
       <c r="E170" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="F170" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G170" s="19">
         <f>E170*60</f>
-        <v>0</v>
+        <v>277.9264</v>
       </c>
       <c r="H170" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I170" s="19">
         <f>E170</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="J170" s="16" t="s">
         <v>16</v>
@@ -10495,21 +10495,21 @@
       </c>
       <c r="E171" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="F171" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G171" s="19">
         <f>E171*60</f>
-        <v>0</v>
+        <v>277.9264</v>
       </c>
       <c r="H171" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I171" s="19">
         <f>E171</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="J171" s="16" t="s">
         <v>16</v>
@@ -10527,21 +10527,21 @@
       </c>
       <c r="E172" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="F172" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G172" s="19">
         <f>E172*60</f>
-        <v>0</v>
+        <v>277.9264</v>
       </c>
       <c r="H172" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I172" s="19">
         <f>E172</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="J172" s="16" t="s">
         <v>16</v>
@@ -10559,7 +10559,7 @@
       <c r="H173" s="15"/>
       <c r="I173" s="15">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>0</v>
+        <v>4.632106666666667</v>
       </c>
       <c r="J173" s="15" t="s">
         <v>17</v>
@@ -10647,21 +10647,21 @@
       </c>
       <c r="E178" s="19">
         <f>($I$119+$I$130+$I$150+$I$163+$I$173)/8</f>
-        <v>0</v>
+        <v>5.3166799999999999</v>
       </c>
       <c r="F178" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G178" s="19">
         <f>E178</f>
-        <v>0</v>
+        <v>5.3166799999999999</v>
       </c>
       <c r="H178" s="16" t="s">
         <v>92</v>
       </c>
       <c r="I178" s="19">
         <f>(G178*C178)/60</f>
-        <v>0</v>
+        <v>0.8861133333333332</v>
       </c>
       <c r="J178" s="16" t="s">
         <v>16</v>
@@ -10679,21 +10679,21 @@
       </c>
       <c r="E179" s="16">
         <f>C7</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F179" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G179" s="16">
         <f>C179*E179</f>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="H179" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I179" s="19">
         <f>G179/60</f>
-        <v>0</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="J179" s="16" t="s">
         <v>16</v>
@@ -10711,21 +10711,21 @@
       </c>
       <c r="E180" s="16">
         <f>EVEN(C6/3)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F180" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G180" s="16" t="b">
+      <c r="G180" s="16">
         <f>IF(I119&gt;0.1,(C180*E180)+25)</f>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H180" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I180" s="19">
         <f>G180/60</f>
-        <v>0</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="J180" s="16" t="s">
         <v>16</v>
@@ -10743,21 +10743,21 @@
       </c>
       <c r="E181" s="19">
         <f>($I$119+$I$130+$I$150+$I$163+$I$173)/8</f>
-        <v>0</v>
+        <v>5.3166799999999999</v>
       </c>
       <c r="F181" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G181" s="19">
         <f>E181</f>
-        <v>0</v>
+        <v>5.3166799999999999</v>
       </c>
       <c r="H181" s="16" t="s">
         <v>92</v>
       </c>
       <c r="I181" s="19">
         <f>(G181*C181)/60</f>
-        <v>0</v>
+        <v>1.32917</v>
       </c>
       <c r="J181" s="16" t="s">
         <v>16</v>
@@ -10775,7 +10775,7 @@
       <c r="H182" s="15"/>
       <c r="I182" s="15">
         <f>SUM(I178:I181)</f>
-        <v>0</v>
+        <v>6.9986166666666669</v>
       </c>
       <c r="J182" s="15" t="s">
         <v>17</v>
@@ -11781,7 +11781,7 @@
       <c r="H220" s="165"/>
       <c r="I220" s="38">
         <f>($G$39+$G$40+$G$41)</f>
-        <v>0</v>
+        <v>69.532056666666676</v>
       </c>
       <c r="J220" s="41"/>
     </row>

</xml_diff>

<commit_message>
Remove Cell Index and Use Range
</commit_message>
<xml_diff>
--- a/ExcelInterop/Assembly_time_calculator.xlsx
+++ b/ExcelInterop/Assembly_time_calculator.xlsx
@@ -2370,7 +2370,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$292" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$292" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6239,7 +6239,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="134">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D6" s="135"/>
       <c r="E6" s="28"/>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="G39" s="72">
         <f>($I$119+$I$130+$I$150+$I$163+$I$193+$I$204+$I$219)+IF($C$13=$B$248,C7*2)</f>
-        <v>57.901333333333334</v>
+        <v>197.43466666666666</v>
       </c>
       <c r="H39" s="145" t="s">
         <v>28</v>
@@ -6997,7 +6997,7 @@
       <c r="I39" s="146"/>
       <c r="J39" s="151">
         <f>SUM(G39:G42)</f>
-        <v>76.485262333333338</v>
+        <v>247.96469744444443</v>
       </c>
       <c r="K39" s="75"/>
       <c r="L39" s="26"/>
@@ -7014,7 +7014,7 @@
       </c>
       <c r="G40" s="73">
         <f>$I$182</f>
-        <v>6.9986166666666669</v>
+        <v>16.141705555555557</v>
       </c>
       <c r="H40" s="147"/>
       <c r="I40" s="148"/>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="G41" s="74">
         <f>$I$173</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="H41" s="147"/>
       <c r="I41" s="148"/>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="G42" s="74">
         <f>($G$39+$G$40+$G$41)*10%</f>
-        <v>6.9532056666666682</v>
+        <v>22.54224522222222</v>
       </c>
       <c r="H42" s="149"/>
       <c r="I42" s="150"/>
@@ -7420,21 +7420,21 @@
       </c>
       <c r="E65" s="16">
         <f>IF(C5=B227,C6,0)</f>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F65" s="76" t="s">
         <v>0</v>
       </c>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
-        <v>468</v>
+        <v>4680</v>
       </c>
       <c r="H65" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I65" s="19">
         <f t="shared" si="1"/>
-        <v>7.8</v>
+        <v>78</v>
       </c>
       <c r="J65" s="16" t="s">
         <v>16</v>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="E71" s="98">
         <f>((C6/C52*1000)*2+2)</f>
-        <v>52</v>
+        <v>502</v>
       </c>
       <c r="F71" s="76" t="s">
         <v>2</v>
@@ -7623,7 +7623,7 @@
       </c>
       <c r="H71" s="98">
         <f>IF(D52&lt;=0,E71)</f>
-        <v>52</v>
+        <v>502</v>
       </c>
       <c r="I71" s="19" t="b">
         <f>IF($D$16=$B$248,(G71+H71)*C71)</f>
@@ -7631,7 +7631,7 @@
       </c>
       <c r="J71" s="157">
         <f>IF(C9=C247,SUM(I71:I73))</f>
-        <v>1.2266666666666668</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7644,7 +7644,7 @@
       </c>
       <c r="E72" s="98">
         <f>IF(C11=B234,0,(((C6/C12)*1000)*2+2))</f>
-        <v>15.333333333333334</v>
+        <v>135.33333333333334</v>
       </c>
       <c r="F72" s="76" t="s">
         <v>2</v>
@@ -7655,11 +7655,11 @@
       </c>
       <c r="H72" s="98">
         <f>IF(D12&lt;=0,E72)</f>
-        <v>15.333333333333334</v>
+        <v>135.33333333333334</v>
       </c>
       <c r="I72" s="19">
         <f>IF($C$11=$B$234,0,(G72+H72)*C72)</f>
-        <v>1.2266666666666668</v>
+        <v>10.826666666666668</v>
       </c>
       <c r="J72" s="158"/>
     </row>
@@ -7673,19 +7673,19 @@
       </c>
       <c r="E73" s="98">
         <f>C6*C73</f>
-        <v>1.2</v>
+        <v>12</v>
       </c>
       <c r="F73" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G73" s="19">
         <f>(E73-I71-I72)</f>
-        <v>-2.6666666666666838E-2</v>
+        <v>1.173333333333332</v>
       </c>
       <c r="H73" s="26"/>
       <c r="I73" s="97">
         <f>IF(G73&gt;0,G73,IF(G73&lt;0,0))</f>
-        <v>0</v>
+        <v>1.173333333333332</v>
       </c>
       <c r="J73" s="159"/>
     </row>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="E74" s="98">
         <f>((C6/C52*1000)*2+2)</f>
-        <v>52</v>
+        <v>502</v>
       </c>
       <c r="F74" s="76" t="s">
         <v>2</v>
@@ -7712,7 +7712,7 @@
       </c>
       <c r="H74" s="98">
         <f>IF(D52&lt;=0,E74)</f>
-        <v>52</v>
+        <v>502</v>
       </c>
       <c r="I74" s="19" t="b">
         <f>IF($D$16=$B$248,(G74+H74)*C74)</f>
@@ -7733,7 +7733,7 @@
       </c>
       <c r="E75" s="98">
         <f>IF(C11=B234,0,(((C6/C12)*1000)*2+2))</f>
-        <v>15.333333333333334</v>
+        <v>135.33333333333334</v>
       </c>
       <c r="F75" s="76" t="s">
         <v>2</v>
@@ -7744,11 +7744,11 @@
       </c>
       <c r="H75" s="98">
         <f>IF(D12&lt;=0,E75)</f>
-        <v>15.333333333333334</v>
+        <v>135.33333333333334</v>
       </c>
       <c r="I75" s="19">
         <f>IF($C$11=$B$234,0,(G75+H75)*C75)</f>
-        <v>0.92</v>
+        <v>8.120000000000001</v>
       </c>
       <c r="J75" s="158"/>
     </row>
@@ -7762,19 +7762,19 @@
       </c>
       <c r="E76" s="98">
         <f>C6*C76</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F76" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G76" s="19">
         <f>(E76-I74-I75)</f>
-        <v>7.999999999999996E-2</v>
+        <v>1.879999999999999</v>
       </c>
       <c r="H76" s="26"/>
       <c r="I76" s="97">
         <f>IF(G76&gt;0,G76,IF(G76&lt;0,0))</f>
-        <v>7.999999999999996E-2</v>
+        <v>1.879999999999999</v>
       </c>
       <c r="J76" s="159"/>
     </row>
@@ -7790,7 +7790,7 @@
       </c>
       <c r="E77" s="98">
         <f>((C6/C52*1000)*2+2)</f>
-        <v>52</v>
+        <v>502</v>
       </c>
       <c r="F77" s="76" t="s">
         <v>2</v>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="H77" s="98">
         <f>IF(D52&lt;=0,E77)</f>
-        <v>52</v>
+        <v>502</v>
       </c>
       <c r="I77" s="19" t="b">
         <f>IF($D$16=$B$248,(G77+H77)*C77)</f>
@@ -7822,7 +7822,7 @@
       </c>
       <c r="E78" s="98">
         <f>IF(C11=B234,0,(((C6/C12)*1000)*2+2))</f>
-        <v>15.333333333333334</v>
+        <v>135.33333333333334</v>
       </c>
       <c r="F78" s="76" t="s">
         <v>2</v>
@@ -7833,11 +7833,11 @@
       </c>
       <c r="H78" s="98">
         <f>IF(D12&lt;=0,E78)</f>
-        <v>15.333333333333334</v>
+        <v>135.33333333333334</v>
       </c>
       <c r="I78" s="19">
         <f>IF($C$11=$B$234,0,(G78+H78)*C78)</f>
-        <v>0.9966666666666667</v>
+        <v>8.7966666666666669</v>
       </c>
       <c r="J78" s="158"/>
     </row>
@@ -7851,19 +7851,19 @@
       </c>
       <c r="E79" s="98">
         <f>C6*C79</f>
-        <v>1.1500000000000001</v>
+        <v>11.5</v>
       </c>
       <c r="F79" s="76" t="s">
         <v>17</v>
       </c>
       <c r="G79" s="19">
         <f>(E79-I77-I78)</f>
-        <v>0.15333333333333343</v>
+        <v>2.7033333333333331</v>
       </c>
       <c r="H79" s="26"/>
       <c r="I79" s="97">
         <f>IF(G79&gt;0,G79,IF(G79&lt;0,0))</f>
-        <v>0.15333333333333343</v>
+        <v>2.7033333333333331</v>
       </c>
       <c r="J79" s="159"/>
     </row>
@@ -7911,14 +7911,14 @@
       </c>
       <c r="E81" s="16">
         <f>IF(C10=B248,C6,0)</f>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F81" s="76" t="s">
         <v>0</v>
       </c>
       <c r="G81" s="19">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>2800</v>
       </c>
       <c r="H81" s="16" t="b">
         <f>IF(C5=B226,G81)</f>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="I81" s="19">
         <f>(G81+H81)/60</f>
-        <v>4.666666666666667</v>
+        <v>46.666666666666664</v>
       </c>
       <c r="J81" s="76" t="s">
         <v>16</v>
@@ -7944,17 +7944,17 @@
       </c>
       <c r="E82" s="19">
         <f t="shared" ref="E82:E101" si="3">IF(B292=TRUE,($C$6/$C$52)*1000,0)</f>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="F82" s="19">
         <f t="shared" ref="F82:F101" si="4">IF($D$52&lt;1,E82)</f>
-        <v>0</v>
-      </c>
-      <c r="G82" s="19" t="b">
+        <v>250</v>
+      </c>
+      <c r="G82" s="19">
         <f t="shared" ref="G82:G83" si="5">IF((C82*F82)&gt;0,C82*F82)</f>
-        <v>0</v>
-      </c>
-      <c r="H82" s="19" t="b">
+        <v>45</v>
+      </c>
+      <c r="H82" s="19">
         <f t="shared" ref="H82:H101" si="6">IF(B292=TRUE,$D$52*C82)</f>
         <v>0</v>
       </c>
@@ -7962,9 +7962,9 @@
         <f t="shared" ref="I82:I102" si="7">IF($D$16=$B$248,G82+H82)</f>
         <v>0</v>
       </c>
-      <c r="J82" s="19" t="b">
+      <c r="J82" s="19">
         <f t="shared" ref="J82:J84" si="8">IF(B292=TRUE,$E$103)</f>
-        <v>0</v>
+        <v>33.333333333333336</v>
       </c>
     </row>
     <row r="83" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8640,13 +8640,13 @@
       <c r="D102" s="181"/>
       <c r="E102" s="181"/>
       <c r="F102" s="182"/>
-      <c r="G102" s="19" t="e">
+      <c r="G102" s="19">
         <f>IF(D52&lt;=0,AVERAGE(G82:G101))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H102" s="19" t="e">
+        <v>45</v>
+      </c>
+      <c r="H102" s="19">
         <f>AVERAGE(H82:H101)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="I102" s="19" t="b">
         <f t="shared" si="7"/>
@@ -8668,15 +8668,15 @@
       </c>
       <c r="E103" s="98">
         <f>($C6/3)</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="F103" s="98" t="e">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="F103" s="98">
         <f>AVERAGE(J82:J101)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G103" s="98" t="e">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="G103" s="98">
         <f>E103+F103</f>
-        <v>#DIV/0!</v>
+        <v>66.666666666666671</v>
       </c>
       <c r="H103" s="76" t="s">
         <v>2</v>
@@ -9068,15 +9068,15 @@
       </c>
       <c r="E116" s="16">
         <f>EVEN(IF(C11=B235,(C6/C12)*1000,0))</f>
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="F116" s="16">
         <f>IF(D12&lt;1,E116)</f>
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="G116" s="16">
         <f>F116*C116</f>
-        <v>2.2080000000000002</v>
+        <v>18.768000000000001</v>
       </c>
       <c r="H116" s="16">
         <f>IF(C11=B235,D12*C116)</f>
@@ -9084,7 +9084,7 @@
       </c>
       <c r="I116" s="19">
         <f>G116+H116</f>
-        <v>2.2080000000000002</v>
+        <v>18.768000000000001</v>
       </c>
       <c r="J116" s="16" t="s">
         <v>16</v>
@@ -9170,7 +9170,7 @@
       <c r="H119" s="15"/>
       <c r="I119" s="15">
         <f>SUM(I63:I70,J71:J79,I80:I81,I102:I103,I114:I118)</f>
-        <v>37.901333333333334</v>
+        <v>177.43466666666666</v>
       </c>
       <c r="J119" s="15" t="s">
         <v>17</v>
@@ -10399,21 +10399,21 @@
       </c>
       <c r="E168" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="F168" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G168" s="19">
         <f>E168*60</f>
-        <v>277.9264</v>
+        <v>710.76479999999992</v>
       </c>
       <c r="H168" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I168" s="19">
         <f>E168</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="J168" s="16" t="s">
         <v>16</v>
@@ -10431,21 +10431,21 @@
       </c>
       <c r="E169" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="F169" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G169" s="19">
         <f>E169*60</f>
-        <v>277.9264</v>
+        <v>710.76479999999992</v>
       </c>
       <c r="H169" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I169" s="19">
         <f>E169</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="J169" s="16" t="s">
         <v>16</v>
@@ -10463,21 +10463,21 @@
       </c>
       <c r="E170" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="F170" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G170" s="19">
         <f>E170*60</f>
-        <v>277.9264</v>
+        <v>710.76479999999992</v>
       </c>
       <c r="H170" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I170" s="19">
         <f>E170</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="J170" s="16" t="s">
         <v>16</v>
@@ -10495,21 +10495,21 @@
       </c>
       <c r="E171" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="F171" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G171" s="19">
         <f>E171*60</f>
-        <v>277.9264</v>
+        <v>710.76479999999992</v>
       </c>
       <c r="H171" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I171" s="19">
         <f>E171</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="J171" s="16" t="s">
         <v>16</v>
@@ -10527,21 +10527,21 @@
       </c>
       <c r="E172" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="F172" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G172" s="19">
         <f>E172*60</f>
-        <v>277.9264</v>
+        <v>710.76479999999992</v>
       </c>
       <c r="H172" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I172" s="19">
         <f>E172</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="J172" s="16" t="s">
         <v>16</v>
@@ -10559,7 +10559,7 @@
       <c r="H173" s="15"/>
       <c r="I173" s="15">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>4.632106666666667</v>
+        <v>11.846079999999999</v>
       </c>
       <c r="J173" s="15" t="s">
         <v>17</v>
@@ -10647,21 +10647,21 @@
       </c>
       <c r="E178" s="19">
         <f>($I$119+$I$130+$I$150+$I$163+$I$173)/8</f>
-        <v>5.3166799999999999</v>
+        <v>23.660093333333332</v>
       </c>
       <c r="F178" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G178" s="19">
         <f>E178</f>
-        <v>5.3166799999999999</v>
+        <v>23.660093333333332</v>
       </c>
       <c r="H178" s="16" t="s">
         <v>92</v>
       </c>
       <c r="I178" s="19">
         <f>(G178*C178)/60</f>
-        <v>0.8861133333333332</v>
+        <v>3.943348888888889</v>
       </c>
       <c r="J178" s="16" t="s">
         <v>16</v>
@@ -10711,21 +10711,21 @@
       </c>
       <c r="E180" s="16">
         <f>EVEN(C6/3)</f>
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F180" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G180" s="16">
         <f>IF(I119&gt;0.1,(C180*E180)+25)</f>
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="H180" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I180" s="19">
         <f>G180/60</f>
-        <v>0.6166666666666667</v>
+        <v>2.1166666666666667</v>
       </c>
       <c r="J180" s="16" t="s">
         <v>16</v>
@@ -10743,21 +10743,21 @@
       </c>
       <c r="E181" s="19">
         <f>($I$119+$I$130+$I$150+$I$163+$I$173)/8</f>
-        <v>5.3166799999999999</v>
+        <v>23.660093333333332</v>
       </c>
       <c r="F181" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G181" s="19">
         <f>E181</f>
-        <v>5.3166799999999999</v>
+        <v>23.660093333333332</v>
       </c>
       <c r="H181" s="16" t="s">
         <v>92</v>
       </c>
       <c r="I181" s="19">
         <f>(G181*C181)/60</f>
-        <v>1.32917</v>
+        <v>5.9150233333333331</v>
       </c>
       <c r="J181" s="16" t="s">
         <v>16</v>
@@ -10775,7 +10775,7 @@
       <c r="H182" s="15"/>
       <c r="I182" s="15">
         <f>SUM(I178:I181)</f>
-        <v>6.9986166666666669</v>
+        <v>16.141705555555557</v>
       </c>
       <c r="J182" s="15" t="s">
         <v>17</v>
@@ -11781,7 +11781,7 @@
       <c r="H220" s="165"/>
       <c r="I220" s="38">
         <f>($G$39+$G$40+$G$41)</f>
-        <v>69.532056666666676</v>
+        <v>225.4224522222222</v>
       </c>
       <c r="J220" s="41"/>
     </row>
@@ -12776,7 +12776,7 @@
     </row>
     <row r="292" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B292" s="42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C292" s="42"/>
       <c r="D292" s="41"/>

</xml_diff>

<commit_message>
App Setting according to Config file
</commit_message>
<xml_diff>
--- a/ExcelInterop/Assembly_time_calculator.xlsx
+++ b/ExcelInterop/Assembly_time_calculator.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="220">
   <si>
     <t>m</t>
   </si>
@@ -692,6 +692,9 @@
   </si>
   <si>
     <t>ASSEMBLY WORK HOURS CALCULATOR ver. 16</t>
+  </si>
+  <si>
+    <t>XLX-X85X-6556565656565</t>
   </si>
 </sst>
 </file>
@@ -2122,12 +2125,162 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2146,15 +2299,6 @@
     <xf numFmtId="0" fontId="28" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2192,147 +2336,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6070,19 +6073,19 @@
     </row>
     <row r="2" spans="1:54" s="24" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="173" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="125"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
+      <c r="J2" s="174"/>
+      <c r="K2" s="174"/>
+      <c r="L2" s="175"/>
       <c r="M2" s="25"/>
       <c r="N2" s="23"/>
       <c r="O2" s="23"/>
@@ -6183,23 +6186,23 @@
     </row>
     <row r="4" spans="1:54" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="176" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="127"/>
-      <c r="D4" s="128"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="178"/>
       <c r="E4" s="26"/>
-      <c r="F4" s="136" t="s">
+      <c r="F4" s="183" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="137"/>
-      <c r="H4" s="138"/>
+      <c r="G4" s="184"/>
+      <c r="H4" s="185"/>
       <c r="I4" s="51"/>
-      <c r="J4" s="129" t="s">
+      <c r="J4" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="130"/>
-      <c r="L4" s="131"/>
+      <c r="K4" s="153"/>
+      <c r="L4" s="154"/>
       <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6207,10 +6210,10 @@
       <c r="B5" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="132" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="133"/>
+      <c r="C5" s="179" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="180"/>
       <c r="E5" s="26"/>
       <c r="F5" s="62" t="s">
         <v>105</v>
@@ -6238,10 +6241,10 @@
       <c r="B6" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="134">
+      <c r="C6" s="181">
         <v>100</v>
       </c>
-      <c r="D6" s="135"/>
+      <c r="D6" s="182"/>
       <c r="E6" s="28"/>
       <c r="F6" s="52" t="s">
         <v>163</v>
@@ -6269,10 +6272,10 @@
       <c r="B7" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C7" s="134">
+      <c r="C7" s="181">
         <v>10</v>
       </c>
-      <c r="D7" s="135"/>
+      <c r="D7" s="182"/>
       <c r="E7" s="26"/>
       <c r="F7" s="52" t="s">
         <v>136</v>
@@ -6300,10 +6303,10 @@
       <c r="B8" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="134">
-        <v>0</v>
-      </c>
-      <c r="D8" s="135"/>
+      <c r="C8" s="181">
+        <v>0</v>
+      </c>
+      <c r="D8" s="182"/>
       <c r="E8" s="94"/>
       <c r="F8" s="52" t="s">
         <v>137</v>
@@ -6331,10 +6334,10 @@
       <c r="B9" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="139" t="s">
+      <c r="C9" s="186" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="140"/>
+      <c r="D9" s="187"/>
       <c r="E9" s="26"/>
       <c r="F9" s="52" t="s">
         <v>189</v>
@@ -6362,10 +6365,10 @@
       <c r="B10" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="139" t="s">
+      <c r="C10" s="186" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="140"/>
+      <c r="D10" s="187"/>
       <c r="E10" s="26"/>
       <c r="F10" s="52" t="s">
         <v>138</v>
@@ -6393,10 +6396,10 @@
       <c r="B11" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="139" t="s">
+      <c r="C11" s="186" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="141"/>
+      <c r="D11" s="188"/>
       <c r="E11" s="26"/>
       <c r="F11" s="52" t="s">
         <v>141</v>
@@ -6445,10 +6448,10 @@
       <c r="B13" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="134" t="s">
+      <c r="C13" s="181" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="135"/>
+      <c r="D13" s="182"/>
       <c r="E13" s="50"/>
       <c r="F13" s="52" t="s">
         <v>143</v>
@@ -6460,11 +6463,11 @@
         <v>0</v>
       </c>
       <c r="I13" s="28"/>
-      <c r="J13" s="142" t="s">
+      <c r="J13" s="189" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="143"/>
-      <c r="L13" s="144"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="191"/>
       <c r="M13" s="36"/>
     </row>
     <row r="14" spans="1:54" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6472,10 +6475,10 @@
       <c r="B14" s="104" t="s">
         <v>210</v>
       </c>
-      <c r="C14" s="121">
+      <c r="C14" s="127">
         <v>10</v>
       </c>
-      <c r="D14" s="122"/>
+      <c r="D14" s="128"/>
       <c r="E14" s="26"/>
       <c r="F14" s="53" t="s">
         <v>140</v>
@@ -6521,10 +6524,10 @@
     </row>
     <row r="16" spans="1:54" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="175" t="s">
+      <c r="B16" s="147" t="s">
         <v>154</v>
       </c>
-      <c r="C16" s="176"/>
+      <c r="C16" s="148"/>
       <c r="D16" s="57" t="s">
         <v>33</v>
       </c>
@@ -6550,11 +6553,11 @@
       <c r="C17" s="23"/>
       <c r="D17" s="34"/>
       <c r="E17" s="26"/>
-      <c r="F17" s="129" t="s">
+      <c r="F17" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="130"/>
-      <c r="H17" s="131"/>
+      <c r="G17" s="153"/>
+      <c r="H17" s="154"/>
       <c r="I17" s="28"/>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
@@ -6577,11 +6580,11 @@
         <v>42</v>
       </c>
       <c r="I18" s="28"/>
-      <c r="J18" s="177" t="s">
+      <c r="J18" s="149" t="s">
         <v>170</v>
       </c>
-      <c r="K18" s="178"/>
-      <c r="L18" s="179"/>
+      <c r="K18" s="150"/>
+      <c r="L18" s="151"/>
       <c r="M18" s="36"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -6626,10 +6629,18 @@
       <c r="H20" s="8">
         <v>0</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="117"/>
-      <c r="K20" s="118"/>
-      <c r="L20" s="56"/>
+      <c r="I20" s="26">
+        <v>100</v>
+      </c>
+      <c r="J20" s="117">
+        <v>100</v>
+      </c>
+      <c r="K20" s="118">
+        <v>101</v>
+      </c>
+      <c r="L20" s="56">
+        <v>102</v>
+      </c>
       <c r="M20" s="36"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -6647,10 +6658,18 @@
       <c r="H21" s="8">
         <v>0</v>
       </c>
-      <c r="I21" s="26"/>
-      <c r="J21" s="117"/>
-      <c r="K21" s="118"/>
-      <c r="L21" s="56"/>
+      <c r="I21" s="26">
+        <v>103</v>
+      </c>
+      <c r="J21" s="117">
+        <v>103</v>
+      </c>
+      <c r="K21" s="118">
+        <v>104</v>
+      </c>
+      <c r="L21" s="56">
+        <v>105</v>
+      </c>
       <c r="M21" s="36"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -6668,10 +6687,18 @@
       <c r="H22" s="8">
         <v>0</v>
       </c>
-      <c r="I22" s="26"/>
-      <c r="J22" s="117"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="56"/>
+      <c r="I22" s="26">
+        <v>106</v>
+      </c>
+      <c r="J22" s="117">
+        <v>106</v>
+      </c>
+      <c r="K22" s="118">
+        <v>107</v>
+      </c>
+      <c r="L22" s="56">
+        <v>108</v>
+      </c>
       <c r="M22" s="36"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -6689,10 +6716,18 @@
       <c r="H23" s="8">
         <v>0</v>
       </c>
-      <c r="I23" s="26"/>
-      <c r="J23" s="117"/>
-      <c r="K23" s="118"/>
-      <c r="L23" s="56"/>
+      <c r="I23" s="26">
+        <v>109</v>
+      </c>
+      <c r="J23" s="117">
+        <v>109</v>
+      </c>
+      <c r="K23" s="118">
+        <v>110</v>
+      </c>
+      <c r="L23" s="56">
+        <v>111</v>
+      </c>
       <c r="M23" s="36"/>
     </row>
     <row r="24" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6710,10 +6745,18 @@
       <c r="H24" s="9">
         <v>0</v>
       </c>
-      <c r="I24" s="28"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="118"/>
-      <c r="L24" s="56"/>
+      <c r="I24" s="28">
+        <v>112</v>
+      </c>
+      <c r="J24" s="117">
+        <v>112</v>
+      </c>
+      <c r="K24" s="118">
+        <v>113</v>
+      </c>
+      <c r="L24" s="56">
+        <v>114</v>
+      </c>
       <c r="M24" s="36"/>
     </row>
     <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6725,10 +6768,18 @@
       <c r="F25" s="26"/>
       <c r="G25" s="26"/>
       <c r="H25" s="27"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="117"/>
-      <c r="K25" s="118"/>
-      <c r="L25" s="56"/>
+      <c r="I25" s="26">
+        <v>115</v>
+      </c>
+      <c r="J25" s="117">
+        <v>115</v>
+      </c>
+      <c r="K25" s="118">
+        <v>116</v>
+      </c>
+      <c r="L25" s="56">
+        <v>117</v>
+      </c>
       <c r="M25" s="36"/>
     </row>
     <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6740,10 +6791,18 @@
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
       <c r="H26" s="27"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="117"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="56"/>
+      <c r="I26" s="26">
+        <v>118</v>
+      </c>
+      <c r="J26" s="117">
+        <v>118</v>
+      </c>
+      <c r="K26" s="118">
+        <v>119</v>
+      </c>
+      <c r="L26" s="56">
+        <v>120</v>
+      </c>
       <c r="M26" s="36"/>
     </row>
     <row r="27" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6752,15 +6811,23 @@
       <c r="C27" s="23"/>
       <c r="D27" s="34"/>
       <c r="E27" s="26"/>
-      <c r="F27" s="154" t="s">
+      <c r="F27" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="155"/>
-      <c r="H27" s="156"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="117"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="56"/>
+      <c r="G27" s="171"/>
+      <c r="H27" s="172"/>
+      <c r="I27" s="28">
+        <v>121</v>
+      </c>
+      <c r="J27" s="117">
+        <v>121</v>
+      </c>
+      <c r="K27" s="118">
+        <v>122</v>
+      </c>
+      <c r="L27" s="56">
+        <v>123</v>
+      </c>
       <c r="M27" s="36"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -6778,10 +6845,18 @@
       <c r="H28" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="I28" s="28"/>
-      <c r="J28" s="117"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="56"/>
+      <c r="I28" s="28">
+        <v>124</v>
+      </c>
+      <c r="J28" s="117">
+        <v>124</v>
+      </c>
+      <c r="K28" s="118">
+        <v>125</v>
+      </c>
+      <c r="L28" s="56">
+        <v>126</v>
+      </c>
       <c r="M28" s="36"/>
     </row>
     <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6799,10 +6874,18 @@
       <c r="H29" s="8">
         <v>0</v>
       </c>
-      <c r="I29" s="28"/>
-      <c r="J29" s="119"/>
-      <c r="K29" s="120"/>
-      <c r="L29" s="99"/>
+      <c r="I29" s="28">
+        <v>127</v>
+      </c>
+      <c r="J29" s="119">
+        <v>127</v>
+      </c>
+      <c r="K29" s="120">
+        <v>128</v>
+      </c>
+      <c r="L29" s="99">
+        <v>129</v>
+      </c>
       <c r="M29" s="36"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -6989,15 +7072,15 @@
       </c>
       <c r="G39" s="72">
         <f>($I$119+$I$130+$I$150+$I$163+$I$193+$I$204+$I$219)+IF($C$13=$B$248,C7*2)</f>
-        <v>197.43466666666666</v>
-      </c>
-      <c r="H39" s="145" t="s">
+        <v>133101.43466666667</v>
+      </c>
+      <c r="H39" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="I39" s="146"/>
-      <c r="J39" s="151">
+      <c r="I39" s="162"/>
+      <c r="J39" s="167">
         <f>SUM(G39:G42)</f>
-        <v>247.96469744444443</v>
+        <v>154125.5873025</v>
       </c>
       <c r="K39" s="75"/>
       <c r="L39" s="26"/>
@@ -7014,11 +7097,11 @@
       </c>
       <c r="G40" s="73">
         <f>$I$182</f>
-        <v>16.141705555555557</v>
-      </c>
-      <c r="H40" s="147"/>
-      <c r="I40" s="148"/>
-      <c r="J40" s="152"/>
+        <v>357.66387500000008</v>
+      </c>
+      <c r="H40" s="163"/>
+      <c r="I40" s="164"/>
+      <c r="J40" s="168"/>
       <c r="K40" s="75"/>
       <c r="L40" s="26"/>
       <c r="M40" s="25"/>
@@ -7034,11 +7117,11 @@
       </c>
       <c r="G41" s="74">
         <f>$I$173</f>
-        <v>11.846079999999999</v>
-      </c>
-      <c r="H41" s="147"/>
-      <c r="I41" s="148"/>
-      <c r="J41" s="152"/>
+        <v>6655.0717333333341</v>
+      </c>
+      <c r="H41" s="163"/>
+      <c r="I41" s="164"/>
+      <c r="J41" s="168"/>
       <c r="K41" s="75"/>
       <c r="L41" s="46"/>
       <c r="M41" s="25"/>
@@ -7054,11 +7137,11 @@
       </c>
       <c r="G42" s="74">
         <f>($G$39+$G$40+$G$41)*10%</f>
-        <v>22.54224522222222</v>
-      </c>
-      <c r="H42" s="149"/>
-      <c r="I42" s="150"/>
-      <c r="J42" s="153"/>
+        <v>14011.417027500001</v>
+      </c>
+      <c r="H42" s="165"/>
+      <c r="I42" s="166"/>
+      <c r="J42" s="169"/>
       <c r="K42" s="75"/>
       <c r="L42" s="46"/>
       <c r="M42" s="25"/>
@@ -7224,10 +7307,10 @@
       <c r="B53" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="121" t="s">
+      <c r="C53" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="122"/>
+      <c r="D53" s="128"/>
       <c r="E53" s="4"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
@@ -7271,54 +7354,54 @@
     <row r="56" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:13" s="23" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:13" s="23" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="185" t="s">
+      <c r="B58" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="186"/>
-      <c r="D58" s="186"/>
-      <c r="E58" s="186"/>
-      <c r="F58" s="186"/>
-      <c r="G58" s="186"/>
-      <c r="H58" s="186"/>
-      <c r="I58" s="186"/>
-      <c r="J58" s="187"/>
+      <c r="C58" s="125"/>
+      <c r="D58" s="125"/>
+      <c r="E58" s="125"/>
+      <c r="F58" s="125"/>
+      <c r="G58" s="125"/>
+      <c r="H58" s="125"/>
+      <c r="I58" s="125"/>
+      <c r="J58" s="126"/>
     </row>
     <row r="59" spans="1:13" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:13" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="160" t="s">
+      <c r="B60" s="121" t="s">
         <v>155</v>
       </c>
-      <c r="C60" s="161"/>
-      <c r="D60" s="161"/>
-      <c r="E60" s="161"/>
-      <c r="F60" s="161"/>
-      <c r="G60" s="161"/>
-      <c r="H60" s="161"/>
-      <c r="I60" s="161"/>
-      <c r="J60" s="162"/>
+      <c r="C60" s="122"/>
+      <c r="D60" s="122"/>
+      <c r="E60" s="122"/>
+      <c r="F60" s="122"/>
+      <c r="G60" s="122"/>
+      <c r="H60" s="122"/>
+      <c r="I60" s="122"/>
+      <c r="J60" s="123"/>
       <c r="L60" s="48"/>
     </row>
     <row r="61" spans="1:13" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="183" t="s">
+      <c r="B61" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="184" t="s">
+      <c r="C61" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="184"/>
-      <c r="E61" s="184" t="s">
+      <c r="D61" s="145"/>
+      <c r="E61" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="184"/>
-      <c r="G61" s="191" t="s">
+      <c r="F61" s="145"/>
+      <c r="G61" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="H61" s="191"/>
-      <c r="I61" s="191"/>
-      <c r="J61" s="191"/>
+      <c r="H61" s="146"/>
+      <c r="I61" s="146"/>
+      <c r="J61" s="146"/>
     </row>
     <row r="62" spans="1:13" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="183"/>
+      <c r="B62" s="155"/>
       <c r="C62" s="14" t="s">
         <v>8</v>
       </c>
@@ -7420,21 +7503,21 @@
       </c>
       <c r="E65" s="16">
         <f>IF(C5=B227,C6,0)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F65" s="76" t="s">
         <v>0</v>
       </c>
       <c r="G65" s="16">
         <f t="shared" si="0"/>
-        <v>4680</v>
+        <v>0</v>
       </c>
       <c r="H65" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I65" s="19">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="J65" s="16" t="s">
         <v>16</v>
@@ -7548,21 +7631,21 @@
       </c>
       <c r="E69" s="16">
         <f>IF(OR(C5=B227,C5=B228,),C7,0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F69" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G69" s="16">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="H69" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I69" s="19">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J69" s="16" t="s">
         <v>16</v>
@@ -7601,7 +7684,7 @@
       </c>
     </row>
     <row r="71" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="188" t="s">
+      <c r="B71" s="135" t="s">
         <v>185</v>
       </c>
       <c r="C71" s="76">
@@ -7629,13 +7712,13 @@
         <f>IF($D$16=$B$248,(G71+H71)*C71)</f>
         <v>0</v>
       </c>
-      <c r="J71" s="157">
+      <c r="J71" s="132">
         <f>IF(C9=C247,SUM(I71:I73))</f>
         <v>12</v>
       </c>
     </row>
     <row r="72" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="189"/>
+      <c r="B72" s="136"/>
       <c r="C72" s="76">
         <v>0.08</v>
       </c>
@@ -7661,10 +7744,10 @@
         <f>IF($C$11=$B$234,0,(G72+H72)*C72)</f>
         <v>10.826666666666668</v>
       </c>
-      <c r="J72" s="158"/>
+      <c r="J72" s="133"/>
     </row>
     <row r="73" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="190"/>
+      <c r="B73" s="137"/>
       <c r="C73" s="76">
         <v>0.12</v>
       </c>
@@ -7687,10 +7770,10 @@
         <f>IF(G73&gt;0,G73,IF(G73&lt;0,0))</f>
         <v>1.173333333333332</v>
       </c>
-      <c r="J73" s="159"/>
+      <c r="J73" s="134"/>
     </row>
     <row r="74" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="188" t="s">
+      <c r="B74" s="135" t="s">
         <v>182</v>
       </c>
       <c r="C74" s="76">
@@ -7718,13 +7801,13 @@
         <f>IF($D$16=$B$248,(G74+H74)*C74)</f>
         <v>0</v>
       </c>
-      <c r="J74" s="157" t="b">
+      <c r="J74" s="132" t="b">
         <f>IF(C9=C248,SUM(I74:I76))</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="189"/>
+      <c r="B75" s="136"/>
       <c r="C75" s="76">
         <v>0.06</v>
       </c>
@@ -7750,10 +7833,10 @@
         <f>IF($C$11=$B$234,0,(G75+H75)*C75)</f>
         <v>8.120000000000001</v>
       </c>
-      <c r="J75" s="158"/>
+      <c r="J75" s="133"/>
     </row>
     <row r="76" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="190"/>
+      <c r="B76" s="137"/>
       <c r="C76" s="18">
         <v>0.1</v>
       </c>
@@ -7776,10 +7859,10 @@
         <f>IF(G76&gt;0,G76,IF(G76&lt;0,0))</f>
         <v>1.879999999999999</v>
       </c>
-      <c r="J76" s="159"/>
+      <c r="J76" s="134"/>
     </row>
     <row r="77" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="188" t="s">
+      <c r="B77" s="135" t="s">
         <v>183</v>
       </c>
       <c r="C77" s="76">
@@ -7807,13 +7890,13 @@
         <f>IF($D$16=$B$248,(G77+H77)*C77)</f>
         <v>0</v>
       </c>
-      <c r="J77" s="157" t="b">
+      <c r="J77" s="132" t="b">
         <f>IF(C9=C249,SUM(I77:I79))</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="189"/>
+      <c r="B78" s="136"/>
       <c r="C78" s="76">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -7839,10 +7922,10 @@
         <f>IF($C$11=$B$234,0,(G78+H78)*C78)</f>
         <v>8.7966666666666669</v>
       </c>
-      <c r="J78" s="158"/>
+      <c r="J78" s="133"/>
     </row>
     <row r="79" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="190"/>
+      <c r="B79" s="137"/>
       <c r="C79" s="76">
         <v>0.115</v>
       </c>
@@ -7865,7 +7948,7 @@
         <f>IF(G79&gt;0,G79,IF(G79&lt;0,0))</f>
         <v>2.7033333333333331</v>
       </c>
-      <c r="J79" s="159"/>
+      <c r="J79" s="134"/>
     </row>
     <row r="80" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="16" t="s">
@@ -8633,13 +8716,13 @@
       </c>
     </row>
     <row r="102" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="180" t="s">
+      <c r="B102" s="129" t="s">
         <v>157</v>
       </c>
-      <c r="C102" s="181"/>
-      <c r="D102" s="181"/>
-      <c r="E102" s="181"/>
-      <c r="F102" s="182"/>
+      <c r="C102" s="130"/>
+      <c r="D102" s="130"/>
+      <c r="E102" s="130"/>
+      <c r="F102" s="131"/>
       <c r="G102" s="19">
         <f>IF(D52&lt;=0,AVERAGE(G82:G101))</f>
         <v>45</v>
@@ -9004,13 +9087,13 @@
       <c r="J113" s="19"/>
     </row>
     <row r="114" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="180" t="s">
+      <c r="B114" s="129" t="s">
         <v>157</v>
       </c>
-      <c r="C114" s="181"/>
-      <c r="D114" s="181"/>
-      <c r="E114" s="181"/>
-      <c r="F114" s="182"/>
+      <c r="C114" s="130"/>
+      <c r="D114" s="130"/>
+      <c r="E114" s="130"/>
+      <c r="F114" s="131"/>
       <c r="G114" s="19" t="e">
         <f>AVERAGE(I104:I113)</f>
         <v>#DIV/0!</v>
@@ -9170,7 +9253,7 @@
       <c r="H119" s="15"/>
       <c r="I119" s="15">
         <f>SUM(I63:I70,J71:J79,I80:I81,I102:I103,I114:I118)</f>
-        <v>177.43466666666666</v>
+        <v>91.434666666666658</v>
       </c>
       <c r="J119" s="15" t="s">
         <v>17</v>
@@ -9189,39 +9272,39 @@
       <c r="J121" s="77"/>
     </row>
     <row r="122" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="160" t="s">
+      <c r="B122" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="C122" s="161"/>
-      <c r="D122" s="161"/>
-      <c r="E122" s="161"/>
-      <c r="F122" s="161"/>
-      <c r="G122" s="161"/>
-      <c r="H122" s="161"/>
-      <c r="I122" s="161"/>
-      <c r="J122" s="162"/>
+      <c r="C122" s="122"/>
+      <c r="D122" s="122"/>
+      <c r="E122" s="122"/>
+      <c r="F122" s="122"/>
+      <c r="G122" s="122"/>
+      <c r="H122" s="122"/>
+      <c r="I122" s="122"/>
+      <c r="J122" s="123"/>
     </row>
     <row r="123" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="168" t="s">
+      <c r="B123" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C123" s="170" t="s">
+      <c r="C123" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D123" s="171"/>
-      <c r="E123" s="170" t="s">
+      <c r="D123" s="141"/>
+      <c r="E123" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F123" s="171"/>
-      <c r="G123" s="172" t="s">
+      <c r="F123" s="141"/>
+      <c r="G123" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H123" s="173"/>
-      <c r="I123" s="173"/>
-      <c r="J123" s="174"/>
+      <c r="H123" s="143"/>
+      <c r="I123" s="143"/>
+      <c r="J123" s="144"/>
     </row>
     <row r="124" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="169"/>
+      <c r="B124" s="139"/>
       <c r="C124" s="14" t="s">
         <v>8</v>
       </c>
@@ -9448,39 +9531,39 @@
       <c r="J132" s="41"/>
     </row>
     <row r="133" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="160" t="s">
+      <c r="B133" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="C133" s="161"/>
-      <c r="D133" s="161"/>
-      <c r="E133" s="161"/>
-      <c r="F133" s="161"/>
-      <c r="G133" s="161"/>
-      <c r="H133" s="161"/>
-      <c r="I133" s="161"/>
-      <c r="J133" s="162"/>
+      <c r="C133" s="122"/>
+      <c r="D133" s="122"/>
+      <c r="E133" s="122"/>
+      <c r="F133" s="122"/>
+      <c r="G133" s="122"/>
+      <c r="H133" s="122"/>
+      <c r="I133" s="122"/>
+      <c r="J133" s="123"/>
     </row>
     <row r="134" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="168" t="s">
+      <c r="B134" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C134" s="170" t="s">
+      <c r="C134" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D134" s="171"/>
-      <c r="E134" s="170" t="s">
+      <c r="D134" s="141"/>
+      <c r="E134" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F134" s="171"/>
-      <c r="G134" s="172" t="s">
+      <c r="F134" s="141"/>
+      <c r="G134" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H134" s="173"/>
-      <c r="I134" s="173"/>
-      <c r="J134" s="174"/>
+      <c r="H134" s="143"/>
+      <c r="I134" s="143"/>
+      <c r="J134" s="144"/>
     </row>
     <row r="135" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="169"/>
+      <c r="B135" s="139"/>
       <c r="C135" s="14" t="s">
         <v>8</v>
       </c>
@@ -9985,39 +10068,39 @@
       <c r="K151" s="41"/>
     </row>
     <row r="152" spans="2:11" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="160" t="s">
+      <c r="B152" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="C152" s="161"/>
-      <c r="D152" s="161"/>
-      <c r="E152" s="161"/>
-      <c r="F152" s="161"/>
-      <c r="G152" s="161"/>
-      <c r="H152" s="161"/>
-      <c r="I152" s="161"/>
-      <c r="J152" s="162"/>
+      <c r="C152" s="122"/>
+      <c r="D152" s="122"/>
+      <c r="E152" s="122"/>
+      <c r="F152" s="122"/>
+      <c r="G152" s="122"/>
+      <c r="H152" s="122"/>
+      <c r="I152" s="122"/>
+      <c r="J152" s="123"/>
     </row>
     <row r="153" spans="2:11" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="168" t="s">
+      <c r="B153" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C153" s="170" t="s">
+      <c r="C153" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D153" s="171"/>
-      <c r="E153" s="170" t="s">
+      <c r="D153" s="141"/>
+      <c r="E153" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F153" s="171"/>
-      <c r="G153" s="172" t="s">
+      <c r="F153" s="141"/>
+      <c r="G153" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H153" s="173"/>
-      <c r="I153" s="173"/>
-      <c r="J153" s="174"/>
+      <c r="H153" s="143"/>
+      <c r="I153" s="143"/>
+      <c r="J153" s="144"/>
     </row>
     <row r="154" spans="2:11" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="169"/>
+      <c r="B154" s="139"/>
       <c r="C154" s="14" t="s">
         <v>8</v>
       </c>
@@ -10329,39 +10412,39 @@
       <c r="J164" s="41"/>
     </row>
     <row r="165" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B165" s="160" t="s">
+      <c r="B165" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="C165" s="161"/>
-      <c r="D165" s="161"/>
-      <c r="E165" s="161"/>
-      <c r="F165" s="161"/>
-      <c r="G165" s="161"/>
-      <c r="H165" s="161"/>
-      <c r="I165" s="161"/>
-      <c r="J165" s="162"/>
+      <c r="C165" s="122"/>
+      <c r="D165" s="122"/>
+      <c r="E165" s="122"/>
+      <c r="F165" s="122"/>
+      <c r="G165" s="122"/>
+      <c r="H165" s="122"/>
+      <c r="I165" s="122"/>
+      <c r="J165" s="123"/>
     </row>
     <row r="166" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="168" t="s">
+      <c r="B166" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C166" s="170" t="s">
+      <c r="C166" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D166" s="171"/>
-      <c r="E166" s="170" t="s">
+      <c r="D166" s="141"/>
+      <c r="E166" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F166" s="171"/>
-      <c r="G166" s="172" t="s">
+      <c r="F166" s="141"/>
+      <c r="G166" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H166" s="173"/>
-      <c r="I166" s="173"/>
-      <c r="J166" s="174"/>
+      <c r="H166" s="143"/>
+      <c r="I166" s="143"/>
+      <c r="J166" s="144"/>
     </row>
     <row r="167" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="169"/>
+      <c r="B167" s="139"/>
       <c r="C167" s="14" t="s">
         <v>8</v>
       </c>
@@ -10399,21 +10482,21 @@
       </c>
       <c r="E168" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="F168" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G168" s="19">
         <f>E168*60</f>
-        <v>710.76479999999992</v>
+        <v>399304.30400000006</v>
       </c>
       <c r="H168" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I168" s="19">
         <f>E168</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="J168" s="16" t="s">
         <v>16</v>
@@ -10431,21 +10514,21 @@
       </c>
       <c r="E169" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="F169" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G169" s="19">
         <f>E169*60</f>
-        <v>710.76479999999992</v>
+        <v>399304.30400000006</v>
       </c>
       <c r="H169" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I169" s="19">
         <f>E169</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="J169" s="16" t="s">
         <v>16</v>
@@ -10463,21 +10546,21 @@
       </c>
       <c r="E170" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="F170" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G170" s="19">
         <f>E170*60</f>
-        <v>710.76479999999992</v>
+        <v>399304.30400000006</v>
       </c>
       <c r="H170" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I170" s="19">
         <f>E170</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="J170" s="16" t="s">
         <v>16</v>
@@ -10495,21 +10578,21 @@
       </c>
       <c r="E171" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="F171" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G171" s="19">
         <f>E171*60</f>
-        <v>710.76479999999992</v>
+        <v>399304.30400000006</v>
       </c>
       <c r="H171" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I171" s="19">
         <f>E171</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="J171" s="16" t="s">
         <v>16</v>
@@ -10527,21 +10610,21 @@
       </c>
       <c r="E172" s="19">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="F172" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G172" s="19">
         <f>E172*60</f>
-        <v>710.76479999999992</v>
+        <v>399304.30400000006</v>
       </c>
       <c r="H172" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I172" s="19">
         <f>E172</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="J172" s="16" t="s">
         <v>16</v>
@@ -10559,7 +10642,7 @@
       <c r="H173" s="15"/>
       <c r="I173" s="15">
         <f>IF($G$39&lt;=0,0,IF($G$39&lt;25,$G$39*$C$168%,IF($G$39&lt;50,$G$39*$C$169%,IF($G$39&lt;100,$G$39*$C$170%,IF($G$39&lt;250,$G$39*$C$171%,IF($G$39&gt;250,$G$39*$C$172%))))))</f>
-        <v>11.846079999999999</v>
+        <v>6655.0717333333341</v>
       </c>
       <c r="J173" s="15" t="s">
         <v>17</v>
@@ -10577,39 +10660,39 @@
       <c r="J174" s="41"/>
     </row>
     <row r="175" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="160" t="s">
+      <c r="B175" s="121" t="s">
         <v>148</v>
       </c>
-      <c r="C175" s="161"/>
-      <c r="D175" s="161"/>
-      <c r="E175" s="161"/>
-      <c r="F175" s="161"/>
-      <c r="G175" s="161"/>
-      <c r="H175" s="161"/>
-      <c r="I175" s="161"/>
-      <c r="J175" s="162"/>
+      <c r="C175" s="122"/>
+      <c r="D175" s="122"/>
+      <c r="E175" s="122"/>
+      <c r="F175" s="122"/>
+      <c r="G175" s="122"/>
+      <c r="H175" s="122"/>
+      <c r="I175" s="122"/>
+      <c r="J175" s="123"/>
     </row>
     <row r="176" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="168" t="s">
+      <c r="B176" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C176" s="170" t="s">
+      <c r="C176" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D176" s="171"/>
-      <c r="E176" s="170" t="s">
+      <c r="D176" s="141"/>
+      <c r="E176" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F176" s="171"/>
-      <c r="G176" s="172" t="s">
+      <c r="F176" s="141"/>
+      <c r="G176" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H176" s="173"/>
-      <c r="I176" s="173"/>
-      <c r="J176" s="174"/>
+      <c r="H176" s="143"/>
+      <c r="I176" s="143"/>
+      <c r="J176" s="144"/>
     </row>
     <row r="177" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="169"/>
+      <c r="B177" s="139"/>
       <c r="C177" s="14" t="s">
         <v>8</v>
       </c>
@@ -10647,21 +10730,21 @@
       </c>
       <c r="E178" s="19">
         <f>($I$119+$I$130+$I$150+$I$163+$I$173)/8</f>
-        <v>23.660093333333332</v>
+        <v>843.31330000000014</v>
       </c>
       <c r="F178" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G178" s="19">
         <f>E178</f>
-        <v>23.660093333333332</v>
+        <v>843.31330000000014</v>
       </c>
       <c r="H178" s="16" t="s">
         <v>92</v>
       </c>
       <c r="I178" s="19">
         <f>(G178*C178)/60</f>
-        <v>3.943348888888889</v>
+        <v>140.55221666666668</v>
       </c>
       <c r="J178" s="16" t="s">
         <v>16</v>
@@ -10743,21 +10826,21 @@
       </c>
       <c r="E181" s="19">
         <f>($I$119+$I$130+$I$150+$I$163+$I$173)/8</f>
-        <v>23.660093333333332</v>
+        <v>843.31330000000014</v>
       </c>
       <c r="F181" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G181" s="19">
         <f>E181</f>
-        <v>23.660093333333332</v>
+        <v>843.31330000000014</v>
       </c>
       <c r="H181" s="16" t="s">
         <v>92</v>
       </c>
       <c r="I181" s="19">
         <f>(G181*C181)/60</f>
-        <v>5.9150233333333331</v>
+        <v>210.82832500000004</v>
       </c>
       <c r="J181" s="16" t="s">
         <v>16</v>
@@ -10775,7 +10858,7 @@
       <c r="H182" s="15"/>
       <c r="I182" s="15">
         <f>SUM(I178:I181)</f>
-        <v>16.141705555555557</v>
+        <v>357.66387500000008</v>
       </c>
       <c r="J182" s="15" t="s">
         <v>17</v>
@@ -10793,39 +10876,39 @@
       <c r="J183" s="41"/>
     </row>
     <row r="184" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="160" t="s">
+      <c r="B184" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="C184" s="161"/>
-      <c r="D184" s="161"/>
-      <c r="E184" s="161"/>
-      <c r="F184" s="161"/>
-      <c r="G184" s="161"/>
-      <c r="H184" s="161"/>
-      <c r="I184" s="161"/>
-      <c r="J184" s="162"/>
+      <c r="C184" s="122"/>
+      <c r="D184" s="122"/>
+      <c r="E184" s="122"/>
+      <c r="F184" s="122"/>
+      <c r="G184" s="122"/>
+      <c r="H184" s="122"/>
+      <c r="I184" s="122"/>
+      <c r="J184" s="123"/>
     </row>
     <row r="185" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="168" t="s">
+      <c r="B185" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C185" s="170" t="s">
+      <c r="C185" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D185" s="171"/>
-      <c r="E185" s="170" t="s">
+      <c r="D185" s="141"/>
+      <c r="E185" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F185" s="171"/>
-      <c r="G185" s="172" t="s">
+      <c r="F185" s="141"/>
+      <c r="G185" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H185" s="173"/>
-      <c r="I185" s="173"/>
-      <c r="J185" s="174"/>
+      <c r="H185" s="143"/>
+      <c r="I185" s="143"/>
+      <c r="J185" s="144"/>
     </row>
     <row r="186" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="169"/>
+      <c r="B186" s="139"/>
       <c r="C186" s="14" t="s">
         <v>8</v>
       </c>
@@ -11073,39 +11156,39 @@
       <c r="J194" s="41"/>
     </row>
     <row r="195" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="160" t="s">
+      <c r="B195" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="C195" s="161"/>
-      <c r="D195" s="161"/>
-      <c r="E195" s="161"/>
-      <c r="F195" s="161"/>
-      <c r="G195" s="161"/>
-      <c r="H195" s="161"/>
-      <c r="I195" s="161"/>
-      <c r="J195" s="162"/>
+      <c r="C195" s="122"/>
+      <c r="D195" s="122"/>
+      <c r="E195" s="122"/>
+      <c r="F195" s="122"/>
+      <c r="G195" s="122"/>
+      <c r="H195" s="122"/>
+      <c r="I195" s="122"/>
+      <c r="J195" s="123"/>
     </row>
     <row r="196" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="168" t="s">
+      <c r="B196" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C196" s="170" t="s">
+      <c r="C196" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D196" s="171"/>
-      <c r="E196" s="170" t="s">
+      <c r="D196" s="141"/>
+      <c r="E196" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F196" s="171"/>
-      <c r="G196" s="172" t="s">
+      <c r="F196" s="141"/>
+      <c r="G196" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H196" s="173"/>
-      <c r="I196" s="173"/>
-      <c r="J196" s="174"/>
+      <c r="H196" s="143"/>
+      <c r="I196" s="143"/>
+      <c r="J196" s="144"/>
     </row>
     <row r="197" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="169"/>
+      <c r="B197" s="139"/>
       <c r="C197" s="14" t="s">
         <v>8</v>
       </c>
@@ -11353,39 +11436,39 @@
       <c r="J205" s="41"/>
     </row>
     <row r="206" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="160" t="s">
+      <c r="B206" s="121" t="s">
         <v>94</v>
       </c>
-      <c r="C206" s="161"/>
-      <c r="D206" s="161"/>
-      <c r="E206" s="161"/>
-      <c r="F206" s="161"/>
-      <c r="G206" s="161"/>
-      <c r="H206" s="161"/>
-      <c r="I206" s="161"/>
-      <c r="J206" s="162"/>
+      <c r="C206" s="122"/>
+      <c r="D206" s="122"/>
+      <c r="E206" s="122"/>
+      <c r="F206" s="122"/>
+      <c r="G206" s="122"/>
+      <c r="H206" s="122"/>
+      <c r="I206" s="122"/>
+      <c r="J206" s="123"/>
     </row>
     <row r="207" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="168" t="s">
+      <c r="B207" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C207" s="170" t="s">
+      <c r="C207" s="140" t="s">
         <v>14</v>
       </c>
-      <c r="D207" s="171"/>
-      <c r="E207" s="170" t="s">
+      <c r="D207" s="141"/>
+      <c r="E207" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="F207" s="171"/>
-      <c r="G207" s="172" t="s">
+      <c r="F207" s="141"/>
+      <c r="G207" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="H207" s="173"/>
-      <c r="I207" s="173"/>
-      <c r="J207" s="174"/>
+      <c r="H207" s="143"/>
+      <c r="I207" s="143"/>
+      <c r="J207" s="144"/>
     </row>
     <row r="208" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="169"/>
+      <c r="B208" s="139"/>
       <c r="C208" s="14" t="s">
         <v>8</v>
       </c>
@@ -11414,32 +11497,32 @@
     <row r="209" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="16">
         <f t="shared" ref="B209:B218" si="29">J20</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C209" s="16">
         <f t="shared" ref="C209:C218" si="30">K20</f>
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D209" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E209" s="16">
         <f t="shared" ref="E209:E218" si="31">L20</f>
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="F209" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G209" s="16">
         <f t="shared" ref="G209:G218" si="32">C209*E209</f>
-        <v>0</v>
+        <v>10302</v>
       </c>
       <c r="H209" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I209" s="19">
         <f>G209</f>
-        <v>0</v>
+        <v>10302</v>
       </c>
       <c r="J209" s="16" t="s">
         <v>16</v>
@@ -11448,32 +11531,32 @@
     <row r="210" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="C210" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D210" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E210" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="F210" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G210" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>10920</v>
       </c>
       <c r="H210" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I210" s="19">
         <f t="shared" ref="I210:I214" si="33">G210</f>
-        <v>0</v>
+        <v>10920</v>
       </c>
       <c r="J210" s="16" t="s">
         <v>16</v>
@@ -11482,32 +11565,32 @@
     <row r="211" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="C211" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="D211" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E211" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="F211" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G211" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>11556</v>
       </c>
       <c r="H211" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I211" s="19">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>11556</v>
       </c>
       <c r="J211" s="16" t="s">
         <v>16</v>
@@ -11516,32 +11599,32 @@
     <row r="212" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="C212" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="D212" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E212" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="F212" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G212" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>12210</v>
       </c>
       <c r="H212" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I212" s="19">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>12210</v>
       </c>
       <c r="J212" s="16" t="s">
         <v>16</v>
@@ -11550,32 +11633,32 @@
     <row r="213" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="C213" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="D213" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E213" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="F213" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G213" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>12882</v>
       </c>
       <c r="H213" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I213" s="19">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>12882</v>
       </c>
       <c r="J213" s="16" t="s">
         <v>16</v>
@@ -11584,32 +11667,32 @@
     <row r="214" spans="2:10" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="C214" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="D214" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E214" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="F214" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G214" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>13572</v>
       </c>
       <c r="H214" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I214" s="19">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>13572</v>
       </c>
       <c r="J214" s="16" t="s">
         <v>16</v>
@@ -11618,32 +11701,32 @@
     <row r="215" spans="2:10" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="C215" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="D215" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E215" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F215" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G215" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>14280</v>
       </c>
       <c r="H215" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I215" s="19">
         <f t="shared" ref="I215:I218" si="34">G215</f>
-        <v>0</v>
+        <v>14280</v>
       </c>
       <c r="J215" s="16" t="s">
         <v>16</v>
@@ -11652,32 +11735,32 @@
     <row r="216" spans="2:10" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B216" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="C216" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="D216" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E216" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="F216" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G216" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>15006</v>
       </c>
       <c r="H216" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I216" s="19">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>15006</v>
       </c>
       <c r="J216" s="16" t="s">
         <v>16</v>
@@ -11686,32 +11769,32 @@
     <row r="217" spans="2:10" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B217" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="C217" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="D217" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E217" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="F217" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G217" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>15750</v>
       </c>
       <c r="H217" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I217" s="19">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>15750</v>
       </c>
       <c r="J217" s="16" t="s">
         <v>16</v>
@@ -11720,32 +11803,32 @@
     <row r="218" spans="2:10" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="16">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C218" s="16">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D218" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E218" s="16">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="F218" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G218" s="16">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>16512</v>
       </c>
       <c r="H218" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I218" s="19">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>16512</v>
       </c>
       <c r="J218" s="16" t="s">
         <v>16</v>
@@ -11763,7 +11846,7 @@
       <c r="H219" s="15"/>
       <c r="I219" s="15">
         <f>SUM(I209:I218)</f>
-        <v>0</v>
+        <v>132990</v>
       </c>
       <c r="J219" s="15" t="s">
         <v>17</v>
@@ -11774,14 +11857,14 @@
       <c r="C220" s="41"/>
       <c r="D220" s="41"/>
       <c r="E220" s="41"/>
-      <c r="F220" s="163" t="s">
+      <c r="F220" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="G220" s="164"/>
-      <c r="H220" s="165"/>
+      <c r="G220" s="157"/>
+      <c r="H220" s="158"/>
       <c r="I220" s="38">
         <f>($G$39+$G$40+$G$41)</f>
-        <v>225.4224522222222</v>
+        <v>140114.17027500001</v>
       </c>
       <c r="J220" s="41"/>
     </row>
@@ -11819,10 +11902,10 @@
       <c r="J223" s="41"/>
     </row>
     <row r="224" spans="2:10" s="23" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="166" t="s">
+      <c r="B224" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="C224" s="167"/>
+      <c r="C224" s="160"/>
       <c r="D224" s="41"/>
       <c r="E224" s="41"/>
       <c r="F224" s="47"/>
@@ -14541,6 +14624,67 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="77">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="H39:I42"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="J74:J76"/>
+    <mergeCell ref="J77:J79"/>
+    <mergeCell ref="B195:J195"/>
+    <mergeCell ref="F220:H220"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B196:B197"/>
+    <mergeCell ref="C196:D196"/>
+    <mergeCell ref="E196:F196"/>
+    <mergeCell ref="G196:J196"/>
+    <mergeCell ref="B206:J206"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="C207:D207"/>
+    <mergeCell ref="E207:F207"/>
+    <mergeCell ref="G207:J207"/>
+    <mergeCell ref="B166:B167"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="E166:F166"/>
+    <mergeCell ref="G166:J166"/>
+    <mergeCell ref="B175:J175"/>
+    <mergeCell ref="G176:J176"/>
+    <mergeCell ref="B184:J184"/>
+    <mergeCell ref="B185:B186"/>
+    <mergeCell ref="C185:D185"/>
+    <mergeCell ref="E185:F185"/>
+    <mergeCell ref="G185:J185"/>
+    <mergeCell ref="B176:B177"/>
+    <mergeCell ref="C176:D176"/>
+    <mergeCell ref="E176:F176"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="E153:F153"/>
+    <mergeCell ref="G153:J153"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="E134:F134"/>
+    <mergeCell ref="G134:J134"/>
+    <mergeCell ref="B152:J152"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B60:J60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:D61"/>
     <mergeCell ref="B165:J165"/>
     <mergeCell ref="B122:J122"/>
     <mergeCell ref="B58:J58"/>
@@ -14557,67 +14701,6 @@
     <mergeCell ref="G123:J123"/>
     <mergeCell ref="E61:F61"/>
     <mergeCell ref="G61:J61"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="E153:F153"/>
-    <mergeCell ref="G153:J153"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="E134:F134"/>
-    <mergeCell ref="G134:J134"/>
-    <mergeCell ref="B152:J152"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B60:J60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="G176:J176"/>
-    <mergeCell ref="B184:J184"/>
-    <mergeCell ref="B185:B186"/>
-    <mergeCell ref="C185:D185"/>
-    <mergeCell ref="E185:F185"/>
-    <mergeCell ref="G185:J185"/>
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="C176:D176"/>
-    <mergeCell ref="E176:F176"/>
-    <mergeCell ref="B166:B167"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="E166:F166"/>
-    <mergeCell ref="G166:J166"/>
-    <mergeCell ref="B175:J175"/>
-    <mergeCell ref="B195:J195"/>
-    <mergeCell ref="F220:H220"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B196:B197"/>
-    <mergeCell ref="C196:D196"/>
-    <mergeCell ref="E196:F196"/>
-    <mergeCell ref="G196:J196"/>
-    <mergeCell ref="B206:J206"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="C207:D207"/>
-    <mergeCell ref="E207:F207"/>
-    <mergeCell ref="G207:J207"/>
-    <mergeCell ref="H39:I42"/>
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="J74:J76"/>
-    <mergeCell ref="J77:J79"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="J13:L13"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21">

</xml_diff>